<commit_message>
Nueva clase para agregar datos
Se agrego una nueva clase que agrega los datos, esto para respetar el principio de responsabilidad única.
</commit_message>
<xml_diff>
--- a/Tutors.xlsx
+++ b/Tutors.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -516,14 +516,29 @@
           <t>Lionel Messi</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>67890543</t>
-        </is>
+      <c r="B6" t="n">
+        <v>67890543</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
           <t>leomessi@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Elton John</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>3456789</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>eltonjohn@gmail.com</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Metodo para agregar tutores
Se agrego el método que agrega tutores
</commit_message>
<xml_diff>
--- a/Tutors.xlsx
+++ b/Tutors.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -531,14 +531,29 @@
           <t>Elton John</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>3456789</t>
-        </is>
+      <c r="B7" t="n">
+        <v>3456789</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
           <t>eltonjohn@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Kanye West</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>5634352</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>kanyewest@gmail.com</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Métodos para agregar tutores y recursos
Se implementaron con contundencia los métodos que sirven para agregar tutores y recursos.
</commit_message>
<xml_diff>
--- a/Tutors.xlsx
+++ b/Tutors.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -546,14 +546,29 @@
           <t>Kanye West</t>
         </is>
       </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>5634352</t>
-        </is>
+      <c r="B8" t="n">
+        <v>5634352</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
           <t>kanyewest@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Will Smith</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>53023029302</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>willsmith@gmail,com</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Mejoras finales entrega 4
Mejoras finales para las entregas finales
</commit_message>
<xml_diff>
--- a/Tutors.xlsx
+++ b/Tutors.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -561,14 +561,29 @@
           <t>Will Smith</t>
         </is>
       </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>53023029302</t>
-        </is>
+      <c r="B9" t="n">
+        <v>53023029302</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
           <t>willsmith@gmail,com</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Pedro Pablo</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>38434734</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>pp@gmail.com</t>
         </is>
       </c>
     </row>

</xml_diff>